<commit_message>
Change the name of a few columns
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\Proyectos\2020_FiscalImpactDecarbonization\4_Model\WORKING_MODEL_FRAMEWORK_July2020\Scenario_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9B31D-B988-459A-B096-2473F6127B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA7EF5C-B5F7-4FDA-A8ED-C9DE4973FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="-13980" windowWidth="17940" windowHeight="12360" tabRatio="864" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>TRYLF</t>
   </si>
   <si>
-    <t>Plain_English</t>
-  </si>
-  <si>
     <t>Electric</t>
   </si>
   <si>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>Tren de Carga</t>
+  </si>
+  <si>
+    <t>Plain English</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -874,12 +874,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -910,17 +908,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,7 +923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,7 +936,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1250,14 +1242,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -1267,112 +1259,112 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
+      <c r="A2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="18"/>
+        <v>89</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1388,7 +1380,7 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1409,13 +1401,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -1433,7 +1425,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>1</v>
@@ -1446,28 +1438,28 @@
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="34" t="s">
+      <c r="B2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1475,24 +1467,24 @@
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18" t="s">
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1500,24 +1492,24 @@
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="18" t="s">
+      <c r="B4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1525,150 +1517,150 @@
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="18" t="s">
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18" t="s">
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="21" t="s">
+      <c r="B11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1696,150 +1688,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="18"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="B8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="18"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="B11" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1851,7 +1843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1862,87 +1856,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C470471-C426-469F-9ED6-2FEDE78EC2A1}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1964,157 +1960,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="27" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D7" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="27" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D8" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="27" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D9" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="27" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D10" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="27" t="s">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2126,7 +2122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3026DB6-0F59-4D5E-A6F2-AAED52E94AFB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2137,157 +2135,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="27" t="s">
+      <c r="B9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="27" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2299,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2311,58 +2309,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="C2" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C3" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2597,9 +2595,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C750AAA-CBE6-4149-8955-F5D689DFF97B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C750AAA-CBE6-4149-8955-F5D689DFF97B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+    <ds:schemaRef ds:uri="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F2A11C5-F080-44F7-BD7A-7F0885D8ED8F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F2A11C5-F080-44F7-BD7A-7F0885D8ED8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adapt B1 and its yaml file to the last RD model. Also, include a litlle module to verified if the solver was add into the neviromental variables in teh main_executer function. Also, put changes teh column Plain_English for Plain English
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/4_Model/RD_Model_v7_Lucía/A1_Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="106_{8D290350-7B29-4947-B92D-E4D9559AD5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89A40EBA-C802-448F-873E-6D6EA17FF947}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA6659F-487A-415B-9AFC-21DE5BFC5564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -49,9 +49,9 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8E173E61-7A36-4940-93D3-48588AAA0DB4}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Correspondería a taxis</t>
       </text>
     </comment>
@@ -143,9 +143,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Plain_English</t>
-  </si>
-  <si>
     <t>Plain Spanish</t>
   </si>
   <si>
@@ -360,13 +357,16 @@
   </si>
   <si>
     <t>Demanda de Transporte - Pasajero Turista</t>
+  </si>
+  <si>
+    <t>Plain English</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,12 +411,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1163,7 +1157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1503,17 +1497,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1533,7 +1527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1545,9 +1539,9 @@
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="52" t="s">
         <v>6</v>
@@ -1557,7 +1551,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="54"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>7</v>
       </c>
@@ -1569,9 +1563,9 @@
       <c r="E4" s="37"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="22" t="s">
@@ -1581,7 +1575,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="39"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1593,9 +1587,9 @@
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
@@ -1605,7 +1599,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1617,7 +1611,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1629,7 +1623,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1641,7 +1635,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1653,7 +1647,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1665,7 +1659,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1694,22 +1688,22 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
@@ -1717,16 +1711,16 @@
         <v>5</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>83</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>84</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>8</v>
@@ -1750,7 +1744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +1775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1816,7 +1810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1849,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1890,7 +1884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1913,7 +1907,7 @@
       </c>
       <c r="M6" s="62"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1934,7 +1928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1953,7 +1947,7 @@
       <c r="L8" s="46"/>
       <c r="M8" s="63"/>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1991,12 +1985,12 @@
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="12.109375" customWidth="1"/>
+    <col min="1" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -2019,7 +2013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -2032,7 +2026,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2045,7 +2039,7 @@
       <c r="F3" s="42"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2058,7 +2052,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2071,7 +2065,7 @@
       <c r="F5" s="42"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -2084,7 +2078,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -2097,7 +2091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2112,7 +2106,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -2137,18 +2131,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
@@ -2156,18 +2150,18 @@
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2176,35 +2170,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
@@ -2215,35 +2209,35 @@
         <v>18</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2256,37 +2250,37 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2295,21 +2289,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2320,77 +2314,77 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2403,197 +2397,197 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="D4" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D6" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="D7" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="D9" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="50" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2605,81 +2599,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2697,6 +2691,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -2927,16 +2931,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
@@ -2946,10 +2940,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2964,4 +2954,23 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chanfge format to create the paths, in that way the path create according the the operational system of the PC
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA6659F-487A-415B-9AFC-21DE5BFC5564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA327A-0EF6-4C00-91EC-3204EB3D753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -1981,7 +1981,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -2131,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2682,25 +2682,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -2931,10 +2912,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2957,20 +2968,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Include some routines forget in the A2 script, also update all data files. Make parametrization of the main yaml file to B1 script and make a little changes to adapt to the JAM energy model. The model generate the same executable input filebut has a little problems with cbc and otoole conection to genereate some results
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\JAM_Model_v1\1_3_4_Ele_Bld_Ind\A1_Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934D99D0-028E-480E-8F2F-8D2F08714B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E973A3A-F27C-40E3-81A6-FC0CFC7DDB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="864" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Plain_English</t>
-  </si>
-  <si>
     <t>Plain Spanish</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>TRXTRAI</t>
+  </si>
+  <si>
+    <t>Plain English</t>
   </si>
 </sst>
 </file>
@@ -599,23 +599,23 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>1</v>
@@ -633,23 +633,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -672,13 +672,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -704,19 +704,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -724,24 +724,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -757,39 +757,39 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -801,42 +801,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3026DB6-0F59-4D5E-A6F2-AAED52E94AFB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -849,36 +851,36 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -887,15 +889,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F74FB0E003A88C4B9D9793633BA4B356" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0b91461ea42f649c0e2a912844849d59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d55314f-45f1-40c9-9fce-63556e193d03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dde1a2dc8a4a80923ccdd7c7b3969d3" ns2:_="">
     <xsd:import namespace="0d55314f-45f1-40c9-9fce-63556e193d03"/>
@@ -1085,6 +1078,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1096,6 +1098,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EDCDF2-89F5-41BC-A27F-AF7AB23C02BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d55314f-45f1-40c9-9fce-63556e193d03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1103,15 +1123,12 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EDCDF2-89F5-41BC-A27F-AF7AB23C02BD}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B95CFD-54EB-415D-BFCA-9AAB4EEFB1B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0d55314f-45f1-40c9-9fce-63556e193d03"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>